<commit_message>
My selenium Project CRM final commit
</commit_message>
<xml_diff>
--- a/CRM_Project/src/test/resources/testdata/CRMData.xlsx
+++ b/CRM_Project/src/test/resources/testdata/CRMData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAKHI\eclipse-workspace\CRM_Project\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAKHI\git\CRMProject\CRM_Project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3FCE0-ECEA-452D-A00F-9129E9F37AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCBA6D5-88B6-4A82-B4F7-10D8ECF65B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -147,10 +147,13 @@
     <t>User is unable to edit project</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>abc1</t>
+    <t>The record has been deleted.</t>
+  </si>
+  <si>
+    <t>projectabc</t>
+  </si>
+  <si>
+    <t>projectabc1</t>
   </si>
 </sst>
 </file>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89920C25-19C3-4369-B47D-54A210235EF9}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +600,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +608,7 @@
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -667,13 +670,16 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
       <c r="J3" t="s">
         <v>28</v>
       </c>
@@ -700,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91381A29-8469-473C-83B8-5F93313A369B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +744,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -750,7 +756,7 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>

</xml_diff>